<commit_message>
created srcipt to add commands to at-commands.mjs file
</commit_message>
<xml_diff>
--- a/tests/menubar-editor/data/200130_Menubar_test_writing.xlsx
+++ b/tests/menubar-editor/data/200130_Menubar_test_writing.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7C7635AE-9F0C-4C55-85FF-1DCADC4CB775}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD241A40-305D-4A40-A248-7473EF0E59C1}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2820" yWindow="2820" windowWidth="21600" windowHeight="11423" firstSheet="3" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3023,8 +3023,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD08FFF1-5FCA-4B3E-93F6-A3BD4D87742D}">
   <dimension ref="A1:J25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1:E1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -3032,9 +3032,10 @@
     <col min="2" max="2" width="65.265625" customWidth="1"/>
     <col min="3" max="3" width="12.1328125" customWidth="1"/>
     <col min="4" max="4" width="38.3984375" customWidth="1"/>
-    <col min="5" max="5" width="11.73046875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.59765625" bestFit="1" customWidth="1"/>
-    <col min="7" max="10" width="11.73046875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="32.265625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14" bestFit="1" customWidth="1"/>
+    <col min="8" max="10" width="11.73046875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">

</xml_diff>